<commit_message>
修改 Signed-off-by: ljj51test <76009075@qq.com>
</commit_message>
<xml_diff>
--- a/用例.xlsx
+++ b/用例.xlsx
@@ -16,13 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>用例1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>用例2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rrrrrr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -367,22 +371,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>11221223</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>